<commit_message>
feat: add content for empty sections; update references.
</commit_message>
<xml_diff>
--- a/bib/referencias.xlsx
+++ b/bib/referencias.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andres/Documents/college/tfg/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ABB24BF-56CB-9644-8D1A-CDC3C62F8A09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBFB244B-471F-5C47-8950-C2FB6402554C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20000" activeTab="2" xr2:uid="{0F6F214A-B5AA-E748-9ABE-129EE0FB3A9D}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="35840" windowHeight="20000" activeTab="2" xr2:uid="{0F6F214A-B5AA-E748-9ABE-129EE0FB3A9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Referencias" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="132">
   <si>
     <t>Problemática</t>
   </si>
@@ -457,6 +457,15 @@
   <si>
     <t>El concepto de microaprendizaje se basa en la curva del olvido de Hermann Ebbinghaus, que establece que cuando las personas absorben grandes cantidades de información, la retención de la misma tiende a disminuir con el tiempo. El microaprendizaje puede utilizarse para abordar este problema. Dividir el contenido en fragmentos pequeños y recordarlos con el tiempo puede mejorar la retención del conocimiento y la productividad. Se pueden utilizar pequeños pasos de aprendizaje, con pequeñas porciones de información, para el aprendizaje intermedio y a demanda. El alumno tiene el control de qué aprende y cuándo. De esta manera, el microaprendizaje permite a los alumnos mantenerse al día en la sociedad del conocimiento actual. El microaprendizaje es un enfoque educativo atractivo para aprender nuevas habilidades e información poco a poco.
 El contenido en línea, como videotutoriales, podcasts de audio, presentaciones, escenarios y evaluaciones, puede presentarse como microaprendizaje. El microaprendizaje no se diferencia mucho de las lecciones tradicionales. En realidad, el microaprendizaje implica condensar y optimizar las lecciones tradicionales para impartirlas en poco tiempo. Este método educativo se centra en el alumno y ofrece formación en tiempo real en múltiples dispositivos (tabletas y teléfonos inteligentes, además de ordenadores de escritorio y portátiles). Cabe destacar que el microaprendizaje podría no ser adecuado para temas más complejos. Si bien es una estrategia de aprendizaje eficaz para reforzar y retener conocimientos, no puede utilizarse para proporcionar conocimientos básicos y profundos, ni para conceptos complejos. El aprendizaje inteligente no es adecuado para desarrollar habilidades analíticas ni para descubrir relaciones de causa y efecto, ya que estas actividades suelen requerir tiempo de planificación y reflexión.</t>
+  </si>
+  <si>
+    <t>Learning Management Systems (LMS) and e-learning management: An integrative review and research agenda</t>
+  </si>
+  <si>
+    <t>La tecnología de la información (TI) puede ser un componente importante para la innovación, ya que posibilita el aprendizaje electrónico y puede proporcionar las condiciones para que una organización pueda trabajar con nuevos negocios y procesos mejorados. En este sentido, los sistemas de gestión del aprendizaje (LMS) permiten la comunicación e interacción entre profesores y estudiantes en espacios virtuales. Sin embargo, la literatura indica que existen lagunas en la investigación, especialmente en lo que respecta al uso de la TI para la gestión del aprendizaje electrónico. El propósito de este documento es analizar la literatura disponible sobre la aplicación de LMS para la gestión del aprendizaje electrónico, buscando presentar posibilidades de investigación en el campo. Se realizó una revisión integradora de la literatura considerando las bases de datos Web of Science, Scopus, Ebsco y Scielo, donde se encontraron 78 referencias, de las cuales 25 fueron artículos completos. Al eliminar la duplicación, quedaron 14 artículos, que llegaron a constituir el portafolio del estudio. El análisis de los artículos permitió concluir que: 1) la estrategia de investigación más frecuente fue la cuantitativa; 2) la encuesta fue el diseño de investigación más utilizado; 3) Las categorías más frecuentes en las plataformas educativas estudiadas pertenecen a Recursos Instruccionales y las menos frecuentes a Interfaz; 4) La mayoría de los estudios se relacionan con el control de la función administrativa; 5) El uso de LMS en la gestión del e-learning aún se debate de forma incipiente en la literatura. Este análisis extrae características interesantes de estudios científicos, destacando lagunas y directrices para futuras investigaciones, incluyendo la analítica del aprendizaje. La principal contribución de este artículo se relaciona con la gestión del e-learning mediante LMS.</t>
+  </si>
+  <si>
+    <t>https://jistem.tecsi.org/index.php/jistem/article/view/10.4301%25S1807-17752016000200001</t>
   </si>
 </sst>
 </file>
@@ -600,6 +609,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -646,12 +661,6 @@
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -666,8 +675,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0F750C0B-658B-E940-88E6-B5432EB62BE2}" name="Table2" displayName="Table2" ref="C3:K28" totalsRowShown="0">
-  <autoFilter ref="C3:K28" xr:uid="{0F750C0B-658B-E940-88E6-B5432EB62BE2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0F750C0B-658B-E940-88E6-B5432EB62BE2}" name="Table2" displayName="Table2" ref="C3:K29" totalsRowShown="0">
+  <autoFilter ref="C3:K29" xr:uid="{0F750C0B-658B-E940-88E6-B5432EB62BE2}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{167E8559-D234-9044-8A82-C54790513719}" name="Link" dataDxfId="7" dataCellStyle="Hyperlink"/>
     <tableColumn id="2" xr3:uid="{7B65CB8B-26A4-174C-86FE-7786243FEE4B}" name="Descripción" dataDxfId="6"/>
@@ -684,10 +693,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{BA4FDF74-9CF3-C04E-8A51-8381BF45087B}" name="Table8" displayName="Table8" ref="B3:B28" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="B3:B28" xr:uid="{BA4FDF74-9CF3-C04E-8A51-8381BF45087B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{BA4FDF74-9CF3-C04E-8A51-8381BF45087B}" name="Table8" displayName="Table8" ref="B3:B29" totalsRowShown="0" dataDxfId="1">
+  <autoFilter ref="B3:B29" xr:uid="{BA4FDF74-9CF3-C04E-8A51-8381BF45087B}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{C7498D62-BD8B-7A44-A415-0CB528647179}" name="Título" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{C7498D62-BD8B-7A44-A415-0CB528647179}" name="Título" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -714,10 +723,10 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C9F82923-E4AB-9046-B830-3ACB5E3D50C4}" name="Table4" displayName="Table4" ref="B2:B8" totalsRowShown="0" dataDxfId="3" dataCellStyle="Hyperlink">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C9F82923-E4AB-9046-B830-3ACB5E3D50C4}" name="Table4" displayName="Table4" ref="B2:B8" totalsRowShown="0" dataDxfId="5" dataCellStyle="Hyperlink">
   <autoFilter ref="B2:B8" xr:uid="{C9F82923-E4AB-9046-B830-3ACB5E3D50C4}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{19C19232-3C73-E145-A36E-A6F8EBDAC59D}" name="Sitios Búsqueda" dataDxfId="2" dataCellStyle="Hyperlink"/>
+    <tableColumn id="1" xr3:uid="{19C19232-3C73-E145-A36E-A6F8EBDAC59D}" name="Sitios Búsqueda" dataDxfId="4" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -734,11 +743,11 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{845D5A3C-0A96-F24A-B66D-8A9A2ACD75CA}" name="Table6" displayName="Table6" ref="B2:C6" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{845D5A3C-0A96-F24A-B66D-8A9A2ACD75CA}" name="Table6" displayName="Table6" ref="B2:C6" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="B2:C6" xr:uid="{845D5A3C-0A96-F24A-B66D-8A9A2ACD75CA}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{0C9E39C6-9978-9640-A59B-20D97D6421EB}" name="Concepto"/>
-    <tableColumn id="2" xr3:uid="{4B40EE62-5C26-1846-A0AF-C0F6456F84B8}" name="Definición" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{4B40EE62-5C26-1846-A0AF-C0F6456F84B8}" name="Definición" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1053,8 +1062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CED00C0-D844-9245-AD35-70AC4C4859F7}">
   <dimension ref="B2:K34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1563,8 +1572,22 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="2:11">
-      <c r="D29" s="5"/>
+    <row r="29" spans="2:11" ht="272">
+      <c r="B29" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="H29" t="s">
+        <v>13</v>
+      </c>
+      <c r="J29" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="32" spans="2:11" ht="34">
       <c r="B32" s="5" t="s">
@@ -1626,11 +1649,16 @@
     <hyperlink ref="C27" r:id="rId13" location="abstract" xr:uid="{6D8CD792-A948-2B4E-8EEE-D492E9D0ABF1}"/>
     <hyperlink ref="C28" r:id="rId14" xr:uid="{F28A5E87-3606-7B42-A414-B6ADEBA15B9E}"/>
     <hyperlink ref="K16" r:id="rId15" xr:uid="{F317A9DC-CA47-F640-AFBB-20F929E7E22F}"/>
+    <hyperlink ref="C6" r:id="rId16" xr:uid="{D1EE4989-3663-DA4D-B162-D258C5B6E34C}"/>
+    <hyperlink ref="C23" r:id="rId17" xr:uid="{FD27A8FE-8B6A-9B4F-9D7B-F018D2FEAC1C}"/>
+    <hyperlink ref="C24" r:id="rId18" xr:uid="{ECD01F1D-BB0A-F04E-8059-D5D98D4A9CDD}"/>
+    <hyperlink ref="C29" r:id="rId19" xr:uid="{A6E990F9-DB7C-7643-AEF6-CF8452B5B681}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="2">
-    <tablePart r:id="rId16"/>
-    <tablePart r:id="rId17"/>
+    <tablePart r:id="rId20"/>
+    <tablePart r:id="rId21"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -1645,13 +1673,13 @@
           <x14:formula1>
             <xm:f>Valores!$D$3</xm:f>
           </x14:formula1>
-          <xm:sqref>E4:I28 E33:I33</xm:sqref>
+          <xm:sqref>E4:I29 E33:I33</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F73A9EC5-506B-0645-BA39-D1DC1EBC3503}">
           <x14:formula1>
             <xm:f>Valores!$B$3:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>J3:J28</xm:sqref>
+          <xm:sqref>J3:J29</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>